<commit_message>
Updates to clearance algorithms
Update includes a successful implementation of the getLandingClearance algorithm. Also removed landing slots at the ports. The takeoff clearance algorithm has a bug.
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/sample_inputs_large.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/sample_inputs_large.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82148199-9F9D-492C-9A54-4707E7E05BC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5041A7DA-B76F-4425-9470-9662070BDAE9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="12300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="12300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operator" sheetId="3" r:id="rId1"/>
@@ -543,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -598,7 +598,7 @@
       </c>
       <c r="B4" s="10">
         <f>B15+B11</f>
-        <v>4800000</v>
+        <v>9300000</v>
       </c>
       <c r="J4" s="19" t="s">
         <v>35</v>
@@ -610,7 +610,7 @@
       </c>
       <c r="B6" s="10">
         <f>B3-B4</f>
-        <v>25200000</v>
+        <v>20700000</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -636,13 +636,13 @@
       </c>
       <c r="B10" s="11">
         <f>C10+D10</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C10" s="13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D10" s="13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -654,7 +654,7 @@
       </c>
       <c r="B11" s="10">
         <f>C10*Aircraft!E2 + D10*Aircraft!E3  + E10*Aircraft!E4</f>
-        <v>4500000</v>
+        <v>9000000</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,7 +886,7 @@
         <v>170</v>
       </c>
       <c r="C2">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>